<commit_message>
1-6 complete and formatted
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicabohannon/Downloads/DA11/Excel/lookups-exercise-jessicabohannon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C0725D-1837-BC49-8F50-03B62A23B91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB8E78F-8B06-D946-AB71-9F7EDF0317DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6020" yWindow="500" windowWidth="29760" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="500" windowWidth="33120" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -826,7 +826,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -839,6 +839,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -914,11 +915,11 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>metro_budget!$B$87</c:f>
+          <c:f>metro_budget!$C$82</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Trustee</c:v>
+              <c:v>Beer Board Budget vs. Actual Spending</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1007,13 +1008,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2451000</c:v>
+                  <c:v>409300</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8925500</c:v>
+                  <c:v>7968300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2321600</c:v>
+                  <c:v>445200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1072,13 +1073,13 @@
                 <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2254684.7999999998</c:v>
+                  <c:v>385908.52</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2204672.88</c:v>
+                  <c:v>427758.64</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2056835.26</c:v>
+                  <c:v>445114.28999999899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1841,12 +1842,12 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1174750</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
       <xdr:row>87</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
@@ -1879,7 +1880,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Paper">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1887,34 +1888,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="444D26"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="FEFAC9"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="A5B592"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="F3A447"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="E7BC29"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="D092A7"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="9C85C0"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="809EC2"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="8E58B6"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="7F6F6F"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -2175,22 +2176,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="D63" sqref="B63:D63"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5" customWidth="1"/>
+    <col min="2" max="4" width="26.5" customWidth="1"/>
     <col min="5" max="5" width="15.83203125" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
-    <col min="8" max="8" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.5" customWidth="1"/>
     <col min="9" max="12" width="15.83203125" customWidth="1"/>
     <col min="13" max="13" width="15.5" customWidth="1"/>
     <col min="14" max="15" width="17.83203125" customWidth="1"/>
-    <col min="16" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -5615,14 +5616,21 @@
         <v>-82077.349999999627</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C82" t="str">
+        <f>_xlfn.CONCAT(B82," Budget vs. Actual Spending")</f>
+        <v>Beer Board Budget vs. Actual Spending</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -5638,12 +5646,12 @@
         <v>73</v>
       </c>
       <c r="B84" s="6">
-        <f>INDEX($B$2:$B$52, MATCH($B$87, A2:$A$52, 0))</f>
-        <v>2451000</v>
+        <f>INDEX($B$2:$B$52, MATCH($B$82, A2:$A$52, 0))</f>
+        <v>409300</v>
       </c>
       <c r="C84" s="6">
-        <f>INDEX($C$2:$C$52, MATCH($B$87, $A$2:$A$52, 0))</f>
-        <v>2254684.7999999998</v>
+        <f>INDEX($C$2:$C$52, MATCH($B$82, $A$2:$A$52, 0))</f>
+        <v>385908.52</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -5651,31 +5659,29 @@
         <v>74</v>
       </c>
       <c r="B85" s="6">
-        <f>INDEX($G$2:$G$52, MATCH($B$87, A3:$A$52, 0))</f>
-        <v>8925500</v>
+        <f>INDEX($G$2:$G$52, MATCH($B$82, A3:$A$52, 0))</f>
+        <v>7968300</v>
       </c>
       <c r="C85" s="6">
-        <f>INDEX($H$2:$H$52, MATCH($B$87, $A$2:$A$52, 0))</f>
-        <v>2204672.88</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+        <f>INDEX($H$2:$H$52, MATCH($B$82, $A$2:$A$52, 0))</f>
+        <v>427758.64</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>75</v>
       </c>
       <c r="B86" s="6">
-        <f>INDEX($L$2:$L$52, MATCH($B$87, $A$2:$A$52, 0))</f>
-        <v>2321600</v>
+        <f>INDEX($L$2:$L$52, MATCH($B$82, $A$2:$A$52, 0))</f>
+        <v>445200</v>
       </c>
       <c r="C86" s="6">
-        <f>INDEX($M$2:$M$52, MATCH($B$87, $A$2:$A$52, 0))</f>
-        <v>2056835.26</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="9" t="s">
-        <v>66</v>
-      </c>
+        <f>INDEX($M$2:$M$52, MATCH($B$82, $A$2:$A$52, 0))</f>
+        <v>445114.28999999899</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B87" s="10"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
@@ -5811,14 +5817,11 @@
       <c r="I100" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83 B87 B82" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87" xr:uid="{59F0A777-5816-3E4F-B02A-28C98D09EF4A}">
-      <formula1>$A$2:$A$52</formula1>
-    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5835,8 +5838,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
1-6 complete, chalenge questions 7a, 8a, 9 complete) git push origin main git status
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicabohannon/Downloads/DA11/Excel/lookups-exercise-jessicabohannon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB8E78F-8B06-D946-AB71-9F7EDF0317DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836B8DC7-3681-4042-B9DE-1AF0B0313010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="500" windowWidth="33120" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1760" yWindow="500" windowWidth="33120" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -826,7 +826,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -839,7 +839,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2176,17 +2175,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.5" customWidth="1"/>
     <col min="2" max="4" width="26.5" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="26.5" customWidth="1"/>
     <col min="9" max="12" width="15.83203125" customWidth="1"/>
     <col min="13" max="13" width="15.5" customWidth="1"/>
@@ -5277,15 +5276,15 @@
         <v>24</v>
       </c>
       <c r="B56">
-        <f>VLOOKUP(A56, $A$2:$E$52, 5)</f>
-        <v>-8.1681998646514792E-2</v>
+        <f>VLOOKUP($A56, $A$2:$P$52, MATCH(B$55, $A$1:$P$1, 0), FALSE)</f>
+        <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f>VLOOKUP(A56, $A$2:$I$52, 9)</f>
+        <f t="shared" ref="C56:D61" si="9">VLOOKUP($A56, $A$2:$P$52, MATCH(C$55, $A$1:$P$1, 0), FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
-        <f>VLOOKUP(A56, $A$2:$N$52, 14)</f>
+        <f t="shared" si="9"/>
         <v>-9181.0800000000163</v>
       </c>
     </row>
@@ -5294,15 +5293,15 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="9">VLOOKUP(A57, $A$2:$E$52, 5)</f>
+        <f t="shared" ref="B57:B61" si="10">VLOOKUP($A57, $A$2:$P$52, MATCH(B$55, $A$1:$P$1, 0), FALSE)</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" ref="C57:C61" si="10">VLOOKUP(A57, $A$2:$I$52, 9)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" ref="D57:D61" si="11">VLOOKUP(A57, $A$2:$N$52, 14)</f>
+        <f t="shared" si="9"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5311,15 +5310,15 @@
         <v>32</v>
       </c>
       <c r="B58">
+        <f t="shared" si="10"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C58">
         <f t="shared" si="9"/>
-        <v>-5.4037002206391245E-2</v>
-      </c>
-      <c r="C58">
-        <f t="shared" si="10"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5328,15 +5327,15 @@
         <v>38</v>
       </c>
       <c r="B59">
+        <f t="shared" si="10"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C59">
         <f t="shared" si="9"/>
-        <v>-1.3334943305713101E-2</v>
-      </c>
-      <c r="C59">
-        <f t="shared" si="10"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5345,15 +5344,15 @@
         <v>39</v>
       </c>
       <c r="B60">
+        <f t="shared" si="10"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C60">
         <f t="shared" si="9"/>
-        <v>-1.0226130964676661E-2</v>
-      </c>
-      <c r="C60">
-        <f t="shared" si="10"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5362,15 +5361,15 @@
         <v>55</v>
       </c>
       <c r="B61">
+        <f t="shared" si="10"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C61">
         <f t="shared" si="9"/>
-        <v>-4.0110550149132493E-2</v>
-      </c>
-      <c r="C61">
-        <f t="shared" si="10"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5398,7 +5397,7 @@
         <v>24</v>
       </c>
       <c r="B65">
-        <f>_xlfn.XLOOKUP(A65, $A$2:$A$52, $D$2:$D$52, FALSE)</f>
+        <f>_xlfn.XLOOKUP($A65, $A$2:$A$52, $D$2:$D$52, FALSE)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C65">
@@ -5415,15 +5414,15 @@
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="12">_xlfn.XLOOKUP(A66, $A$2:$A$52, $D$2:$D$52, FALSE)</f>
+        <f t="shared" ref="B66:B70" si="11">_xlfn.XLOOKUP(A66, $A$2:$A$52, $D$2:$D$52, FALSE)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="13">_xlfn.XLOOKUP(A66, $A$2:$A$52, $I$2:$I$52, FALSE)</f>
+        <f t="shared" ref="C66:C70" si="12">_xlfn.XLOOKUP(A66, $A$2:$A$52, $I$2:$I$52, FALSE)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="14">_xlfn.XLOOKUP(A66, $A$2:$A$52, $N$2:$N$52, FALSE)</f>
+        <f t="shared" ref="D66:D70" si="13">_xlfn.XLOOKUP(A66, $A$2:$A$52, $N$2:$N$52, FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5432,15 +5431,15 @@
         <v>32</v>
       </c>
       <c r="B67">
+        <f t="shared" si="11"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C67">
         <f t="shared" si="12"/>
-        <v>-149396.10000000987</v>
-      </c>
-      <c r="C67">
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D67">
         <f t="shared" si="13"/>
-        <v>-189254.06000000006</v>
-      </c>
-      <c r="D67">
-        <f t="shared" si="14"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5449,15 +5448,15 @@
         <v>38</v>
       </c>
       <c r="B68">
+        <f t="shared" si="11"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C68">
         <f t="shared" si="12"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="C68">
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D68">
         <f t="shared" si="13"/>
-        <v>-45485.580000000075</v>
-      </c>
-      <c r="D68">
-        <f t="shared" si="14"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5466,15 +5465,15 @@
         <v>39</v>
       </c>
       <c r="B69">
+        <f t="shared" si="11"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C69">
         <f t="shared" si="12"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="C69">
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D69">
         <f t="shared" si="13"/>
-        <v>-8005.7900000010268</v>
-      </c>
-      <c r="D69">
-        <f t="shared" si="14"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5483,15 +5482,15 @@
         <v>55</v>
       </c>
       <c r="B70">
+        <f t="shared" si="11"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C70">
         <f t="shared" si="12"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="C70">
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D70">
         <f t="shared" si="13"/>
-        <v>-133456.33000001032</v>
-      </c>
-      <c r="D70">
-        <f t="shared" si="14"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5519,7 +5518,7 @@
         <v>24</v>
       </c>
       <c r="B74">
-        <f>INDEX($D$2:$D$52, MATCH(A74, $A$2:$A$52, 0))</f>
+        <f>INDEX($D$2:$D$52, MATCH($A74, $A$2:$A$52, 0))</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C74">
@@ -5536,15 +5535,15 @@
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="15">INDEX($D$2:$D$52, MATCH(A75, $A$2:$A$52, 0))</f>
+        <f t="shared" ref="B75:B79" si="14">INDEX($D$2:$D$52, MATCH(A75, $A$2:$A$52, 0))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="16">INDEX($I$2:$I$52, MATCH(A75, $A$2:$A$52, 0))</f>
+        <f t="shared" ref="C75:C79" si="15">INDEX($I$2:$I$52, MATCH(A75, $A$2:$A$52, 0))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="17">INDEX($N$2:$N$52, MATCH(A75, $A$2:$A$52, 0))</f>
+        <f t="shared" ref="D75:D79" si="16">INDEX($N$2:$N$52, MATCH(A75, $A$2:$A$52, 0))</f>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5553,15 +5552,15 @@
         <v>32</v>
       </c>
       <c r="B76">
+        <f t="shared" si="14"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="C76">
         <f t="shared" si="15"/>
-        <v>-149396.10000000987</v>
-      </c>
-      <c r="C76">
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="D76">
         <f t="shared" si="16"/>
-        <v>-189254.06000000006</v>
-      </c>
-      <c r="D76">
-        <f t="shared" si="17"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5570,15 +5569,15 @@
         <v>38</v>
       </c>
       <c r="B77">
+        <f t="shared" si="14"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="C77">
         <f t="shared" si="15"/>
-        <v>-12230.810000000056</v>
-      </c>
-      <c r="C77">
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="D77">
         <f t="shared" si="16"/>
-        <v>-45485.580000000075</v>
-      </c>
-      <c r="D77">
-        <f t="shared" si="17"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5587,15 +5586,15 @@
         <v>39</v>
       </c>
       <c r="B78">
+        <f t="shared" si="14"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="C78">
         <f t="shared" si="15"/>
-        <v>-4950.4699999999721</v>
-      </c>
-      <c r="C78">
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="D78">
         <f t="shared" si="16"/>
-        <v>-8005.7900000010268</v>
-      </c>
-      <c r="D78">
-        <f t="shared" si="17"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5604,15 +5603,15 @@
         <v>55</v>
       </c>
       <c r="B79">
+        <f t="shared" si="14"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="C79">
         <f t="shared" si="15"/>
-        <v>-184239.79000001028</v>
-      </c>
-      <c r="C79">
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="D79">
         <f t="shared" si="16"/>
-        <v>-133456.33000001032</v>
-      </c>
-      <c r="D79">
-        <f t="shared" si="17"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5680,9 +5679,6 @@
         <v>445114.28999999899</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B87" s="10"/>
-    </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>76</v>
@@ -5728,25 +5724,88 @@
       <c r="A91" t="s">
         <v>73</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="E91" s="5"/>
-      <c r="G91" s="5"/>
+      <c r="B91" t="str">
+        <f>_xlfn.XLOOKUP(B$89, $F$2:$F$52, $A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C91">
+        <f>_xlfn.XLOOKUP(B$89, $F$2:$F$52, $E$2:$E$52)</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D91" t="str">
+        <f>_xlfn.XLOOKUP(D$89, $F$2:$F$52, $A$2:$A$52)</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E91">
+        <f>_xlfn.XLOOKUP(D$89, $F$2:$F$52, $E$2:$E$52)</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F91" t="str">
+        <f>_xlfn.XLOOKUP(F$89, $F$2:$F$52, $A$2:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G91">
+        <f>_xlfn.XLOOKUP(F$89, $F$2:$F$52, $E$2:$E$52)</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>74</v>
       </c>
-      <c r="C92" s="5"/>
-      <c r="E92" s="5"/>
-      <c r="G92" s="5"/>
+      <c r="B92" t="str">
+        <f>_xlfn.XLOOKUP(B$89, $K$2:$K$52, $A$2:$A$52)</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C92">
+        <f>_xlfn.XLOOKUP(B$89, $F$2:$F$52, $J$2:$J$52)</f>
+        <v>-0.13000189224870184</v>
+      </c>
+      <c r="D92" t="str">
+        <f>_xlfn.XLOOKUP(D$89, $K$2:$K$52, $A$2:$A$52)</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E92">
+        <f>_xlfn.XLOOKUP(D$89, $F$2:$F$52, $J$2:$J$52)</f>
+        <v>-0.10009631366303927</v>
+      </c>
+      <c r="F92" t="str">
+        <f>_xlfn.XLOOKUP(F$89, $K$2:$K$52, $A$2:$A$52)</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G92">
+        <f>_xlfn.XLOOKUP(F$89, $F$2:$F$52, $J$2:$J$52)</f>
+        <v>-0.17103239309050916</v>
+      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>75</v>
       </c>
-      <c r="C93" s="5"/>
-      <c r="E93" s="5"/>
-      <c r="G93" s="5"/>
+      <c r="B93" t="str">
+        <f>_xlfn.XLOOKUP(B$89, $P$2:$P$52, $A$2:$A$52)</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C93">
+        <f>_xlfn.XLOOKUP(B$89, $F$2:$F$52, $O$2:$O$52)</f>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="D93" t="str">
+        <f>_xlfn.XLOOKUP(D$89, $P$2:$P$52, $A$2:$A$52)</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E93">
+        <f>_xlfn.XLOOKUP(D$89, $F$2:$F$52, $O$2:$O$52)</f>
+        <v>-0.11920361114432618</v>
+      </c>
+      <c r="F93" t="str">
+        <f>_xlfn.XLOOKUP(F$89, $P$2:$P$52, $A$2:$A$52)</f>
+        <v>Election Commission</v>
+      </c>
+      <c r="G93">
+        <f>_xlfn.XLOOKUP(F$89, $F$2:$F$52, $O$2:$O$52)</f>
+        <v>-8.6909325643882263E-2</v>
+      </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
@@ -5793,27 +5852,90 @@
       <c r="A98" t="s">
         <v>73</v>
       </c>
-      <c r="C98" s="4"/>
-      <c r="E98" s="4"/>
-      <c r="G98" s="4"/>
+      <c r="B98" t="str">
+        <f>INDEX($A$2:$A$52, MATCH(B$96, $F$2:$F$52, 0))</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="C98">
+        <f>INDEX($E$2:$E$52, MATCH(B$96, $F$2:$F$52, 0))</f>
+        <v>-0.15235918433091292</v>
+      </c>
+      <c r="D98" t="str">
+        <f>INDEX($A$2:$A$52, MATCH(D$96, $F$2:$F$52, 0))</f>
+        <v>Circuit Court Clerk</v>
+      </c>
+      <c r="E98">
+        <f>INDEX($E$2:$E$52, MATCH(D$96, $F$2:$F$52, 0))</f>
+        <v>-0.11502817362571344</v>
+      </c>
+      <c r="F98" t="str">
+        <f>INDEX($A$2:$A$52, MATCH(F$96, $F$2:$F$52, 0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="G98">
+        <f>INDEX($E$2:$E$52, MATCH(F$96, $F$2:$F$52, 0))</f>
+        <v>-9.5782760864849215E-2</v>
+      </c>
       <c r="I98" s="4"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>74</v>
       </c>
-      <c r="C99" s="4"/>
-      <c r="E99" s="4"/>
-      <c r="G99" s="4"/>
+      <c r="B99" t="str">
+        <f>INDEX($A$2:$A$52, MATCH(B$96, $K$2:$K$52, 0))</f>
+        <v>Metropolitan Clerk</v>
+      </c>
+      <c r="C99">
+        <f>INDEX($J$2:$J$52, MATCH(B$96, $F$2:$F$52, 0))</f>
+        <v>-0.13000189224870184</v>
+      </c>
+      <c r="D99" t="str">
+        <f>INDEX($A$2:$A$52, MATCH(D$96, $K$2:$K$52, 0))</f>
+        <v>Internal Audit</v>
+      </c>
+      <c r="E99">
+        <f>INDEX($J$2:$J$52, MATCH(D$96, $F$2:$F$52, 0))</f>
+        <v>-0.10009631366303927</v>
+      </c>
+      <c r="F99" t="str">
+        <f>INDEX($A$2:$A$52, MATCH(F$96, $K$2:$K$52, 0))</f>
+        <v>Office of Family Safety</v>
+      </c>
+      <c r="G99">
+        <f>INDEX($J$2:$J$52, MATCH(F$96, $F$2:$F$52, 0))</f>
+        <v>-0.17103239309050916</v>
+      </c>
       <c r="I99" s="4"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>75</v>
       </c>
-      <c r="C100" s="4"/>
-      <c r="E100" s="4"/>
-      <c r="G100" s="4"/>
+      <c r="B100" t="str">
+        <f>INDEX($A$2:$A$52, MATCH(B$96, $P$2:$P$52, 0))</f>
+        <v>Community Oversight Board</v>
+      </c>
+      <c r="C100">
+        <f>INDEX($O$2:$O$52, MATCH(B$96, $F$2:$F$52, 0))</f>
+        <v>-0.15295680364719175</v>
+      </c>
+      <c r="D100" t="str">
+        <f>INDEX($A$2:$A$52, MATCH(D$96, $P$2:$P$52, 0))</f>
+        <v>Clerk and Master - Chancery</v>
+      </c>
+      <c r="E100">
+        <f>INDEX($O$2:$O$52, MATCH(D$96, $F$2:$F$52, 0))</f>
+        <v>-0.11920361114432618</v>
+      </c>
+      <c r="F100" t="str">
+        <f>INDEX($A$2:$A$52, MATCH(F$96, $P$2:$P$52, 0))</f>
+        <v>Election Commission</v>
+      </c>
+      <c r="G100">
+        <f>INDEX($O$2:$O$52, MATCH(F$96, $F$2:$F$52, 0))</f>
+        <v>-8.6909325643882263E-2</v>
+      </c>
       <c r="I100" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
just need to do 8b
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicabohannon/Downloads/DA11/Excel/lookups-exercise-jessicabohannon/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836B8DC7-3681-4042-B9DE-1AF0B0313010}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDC1FBD-2919-0A49-9924-49F38C332331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1760" yWindow="500" windowWidth="33120" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,8 +33,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="93">
   <si>
     <t>Department</t>
   </si>
@@ -304,6 +326,15 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>Question 7.3</t>
+  </si>
+  <si>
+    <t>Question 7.4</t>
+  </si>
+  <si>
+    <t>Question 7.5</t>
   </si>
 </sst>
 </file>
@@ -826,7 +857,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -839,6 +870,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1839,16 +1872,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>876300</xdr:colOff>
-      <xdr:row>87</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2175,8 +2208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="K69" sqref="K69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5256,6 +5289,9 @@
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="F54" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
@@ -5268,6 +5304,18 @@
         <v>8</v>
       </c>
       <c r="D55" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I55" s="1" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5276,14 +5324,29 @@
         <v>24</v>
       </c>
       <c r="B56">
-        <f>VLOOKUP($A56, $A$2:$P$52, MATCH(B$55, $A$1:$P$1, 0), FALSE)</f>
+        <f>VLOOKUP($A56, $A$2:$P$52, 4, FALSE)</f>
         <v>-36209.630000000005</v>
       </c>
       <c r="C56">
-        <f t="shared" ref="C56:D61" si="9">VLOOKUP($A56, $A$2:$P$52, MATCH(C$55, $A$1:$P$1, 0), FALSE)</f>
+        <f>VLOOKUP($A56, $A$2:$P$52, 9, FALSE)</f>
         <v>-27292.159999999974</v>
       </c>
       <c r="D56">
+        <f>VLOOKUP($A56, $A$2:$P$52, 14, FALSE)</f>
+        <v>-9181.0800000000163</v>
+      </c>
+      <c r="F56" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56">
+        <f>VLOOKUP($A56, $A$2:$P$52, MATCH(G$55, $1:$1, 0), FALSE)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="H56">
+        <f t="shared" ref="H56:I56" si="9">VLOOKUP($A56, $A$2:$P$52, MATCH(H$55, $1:$1, 0), FALSE)</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="I56">
         <f t="shared" si="9"/>
         <v>-9181.0800000000163</v>
       </c>
@@ -5293,15 +5356,30 @@
         <v>25</v>
       </c>
       <c r="B57">
-        <f t="shared" ref="B57:B61" si="10">VLOOKUP($A57, $A$2:$P$52, MATCH(B$55, $A$1:$P$1, 0), FALSE)</f>
+        <f t="shared" ref="B57:B61" si="10">VLOOKUP($A57, $A$2:$P$52, 4, FALSE)</f>
         <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="C57:C61" si="11">VLOOKUP($A57, $A$2:$P$52, 9, FALSE)</f>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="D57:D61" si="12">VLOOKUP($A57, $A$2:$P$52, 14, FALSE)</f>
+        <v>-311228.08999999997</v>
+      </c>
+      <c r="F57" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57">
+        <f t="shared" ref="G57:I61" si="13">VLOOKUP($A57, $A$2:$P$52, MATCH(G$55, $1:$1, 0), FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="13"/>
         <v>-311228.08999999997</v>
       </c>
     </row>
@@ -5314,11 +5392,26 @@
         <v>-149396.10000000987</v>
       </c>
       <c r="C58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
+        <v>-374962.91000000015</v>
+      </c>
+      <c r="F58" t="s">
+        <v>32</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="13"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="13"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="13"/>
         <v>-374962.91000000015</v>
       </c>
     </row>
@@ -5331,11 +5424,26 @@
         <v>-12230.810000000056</v>
       </c>
       <c r="C59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
+        <v>-72.879999999888241</v>
+      </c>
+      <c r="F59" t="s">
+        <v>38</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="13"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="13"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="13"/>
         <v>-72.879999999888241</v>
       </c>
     </row>
@@ -5348,11 +5456,26 @@
         <v>-4950.4699999999721</v>
       </c>
       <c r="C60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
+        <v>-1724.9000000000233</v>
+      </c>
+      <c r="F60" t="s">
+        <v>39</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="13"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="13"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="13"/>
         <v>-1724.9000000000233</v>
       </c>
     </row>
@@ -5365,11 +5488,26 @@
         <v>-184239.79000001028</v>
       </c>
       <c r="C61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="F61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="13"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="13"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="13"/>
         <v>-82077.349999999627</v>
       </c>
     </row>
@@ -5377,6 +5515,9 @@
       <c r="A63" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="F63" s="7" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
@@ -5391,8 +5532,20 @@
       <c r="D64" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>24</v>
       </c>
@@ -5408,98 +5561,199 @@
         <f>_xlfn.XLOOKUP(A65, $A$2:$A$52, $N$2:$N$52, FALSE)</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F65" t="s">
+        <v>24</v>
+      </c>
+      <c r="G65" s="10" cm="1">
+        <f t="array" ref="G65">_xlfn.XLOOKUP($F65,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="H65" s="10" cm="1">
+        <f t="array" ref="H65">_xlfn.XLOOKUP($F65,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(H$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="I65" s="10" cm="1">
+        <f t="array" ref="I65">_xlfn.XLOOKUP($F65,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(I$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="11">_xlfn.XLOOKUP(A66, $A$2:$A$52, $D$2:$D$52, FALSE)</f>
+        <f t="shared" ref="B66:B70" si="14">_xlfn.XLOOKUP(A66, $A$2:$A$52, $D$2:$D$52, FALSE)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ref="C66:C70" si="12">_xlfn.XLOOKUP(A66, $A$2:$A$52, $I$2:$I$52, FALSE)</f>
+        <f t="shared" ref="C66:C70" si="15">_xlfn.XLOOKUP(A66, $A$2:$A$52, $I$2:$I$52, FALSE)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" ref="D66:D70" si="13">_xlfn.XLOOKUP(A66, $A$2:$A$52, $N$2:$N$52, FALSE)</f>
+        <f t="shared" ref="D66:D70" si="16">_xlfn.XLOOKUP(A66, $A$2:$A$52, $N$2:$N$52, FALSE)</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G66" s="10" cm="1">
+        <f t="array" ref="G66">_xlfn.XLOOKUP($F66,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="H66" s="10" cm="1">
+        <f t="array" ref="H66">_xlfn.XLOOKUP($F66,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(H$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="I66" s="10" cm="1">
+        <f t="array" ref="I66">_xlfn.XLOOKUP($F66,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(I$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>32</v>
       </c>
       <c r="B67">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F67" t="s">
+        <v>32</v>
+      </c>
+      <c r="G67" s="10" cm="1">
+        <f t="array" ref="G67">_xlfn.XLOOKUP($F67,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="H67" s="10" cm="1">
+        <f t="array" ref="H67">_xlfn.XLOOKUP($F67,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(H$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="I67" s="10" cm="1">
+        <f t="array" ref="I67">_xlfn.XLOOKUP($F67,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(I$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>38</v>
       </c>
       <c r="B68">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F68" t="s">
+        <v>38</v>
+      </c>
+      <c r="G68" s="10" cm="1">
+        <f t="array" ref="G68">_xlfn.XLOOKUP($F68,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="H68" s="10" cm="1">
+        <f t="array" ref="H68">_xlfn.XLOOKUP($F68,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(H$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="I68" s="10" cm="1">
+        <f t="array" ref="I68">_xlfn.XLOOKUP($F68,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(I$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>39</v>
       </c>
       <c r="B69">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F69" t="s">
+        <v>39</v>
+      </c>
+      <c r="G69" s="10" cm="1">
+        <f t="array" ref="G69">_xlfn.XLOOKUP($F69,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="H69" s="10" cm="1">
+        <f t="array" ref="H69">_xlfn.XLOOKUP($F69,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(H$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="I69" s="10" cm="1">
+        <f t="array" ref="I69">_xlfn.XLOOKUP($F69,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(I$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>55</v>
       </c>
       <c r="B70">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>-82077.349999999627</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F70" t="s">
+        <v>55</v>
+      </c>
+      <c r="G70" s="10" cm="1">
+        <f t="array" ref="G70">_xlfn.XLOOKUP($F70,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(G$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="H70" s="10" cm="1">
+        <f t="array" ref="H70">_xlfn.XLOOKUP($F70,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(H$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="I70" s="10" cm="1">
+        <f t="array" ref="I70">_xlfn.XLOOKUP($F70,$A$1:$A$52,INDEX($A$1:$P$52,,MATCH(I$55,$A$1:$P$1,0)),FALSE)</f>
+        <v>-82077.349999999627</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F72" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -5512,8 +5766,20 @@
       <c r="D73" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H73" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I73" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -5529,89 +5795,179 @@
         <f>INDEX($N$2:$N$52, MATCH(A74, $A$2:$A$52, 0))</f>
         <v>-9181.0800000000163</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F74" t="s">
+        <v>24</v>
+      </c>
+      <c r="G74" s="10">
+        <f>INDEX($A$1:$P$52,MATCH($F74,$A$1:$A$52,0),MATCH(G$73,$A$1:$P$1,0))</f>
+        <v>-36209.630000000005</v>
+      </c>
+      <c r="H74" s="10">
+        <f t="shared" ref="H74:I74" si="17">INDEX($A$1:$P$52,MATCH($F74,$A$1:$A$52,0),MATCH(H$73,$A$1:$P$1,0))</f>
+        <v>-27292.159999999974</v>
+      </c>
+      <c r="I74" s="10">
+        <f t="shared" si="17"/>
+        <v>-9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="14">INDEX($D$2:$D$52, MATCH(A75, $A$2:$A$52, 0))</f>
+        <f t="shared" ref="B75:B79" si="18">INDEX($D$2:$D$52, MATCH(A75, $A$2:$A$52, 0))</f>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" ref="C75:C79" si="15">INDEX($I$2:$I$52, MATCH(A75, $A$2:$A$52, 0))</f>
+        <f t="shared" ref="C75:C79" si="19">INDEX($I$2:$I$52, MATCH(A75, $A$2:$A$52, 0))</f>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" ref="D75:D79" si="16">INDEX($N$2:$N$52, MATCH(A75, $A$2:$A$52, 0))</f>
+        <f t="shared" ref="D75:D79" si="20">INDEX($N$2:$N$52, MATCH(A75, $A$2:$A$52, 0))</f>
         <v>-311228.08999999997</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F75" t="s">
+        <v>25</v>
+      </c>
+      <c r="G75" s="10">
+        <f t="shared" ref="G75:I79" si="21">INDEX($A$1:$P$52,MATCH($F75,$A$1:$A$52,0),MATCH(G$73,$A$1:$P$1,0))</f>
+        <v>0</v>
+      </c>
+      <c r="H75" s="10">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I75" s="10">
+        <f t="shared" si="21"/>
+        <v>-311228.08999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>-189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>-374962.91000000015</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F76" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76" s="10">
+        <f t="shared" si="21"/>
+        <v>-149396.10000000987</v>
+      </c>
+      <c r="H76" s="10">
+        <f t="shared" si="21"/>
+        <v>-189254.06000000006</v>
+      </c>
+      <c r="I76" s="10">
+        <f t="shared" si="21"/>
+        <v>-374962.91000000015</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>-45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>-72.879999999888241</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F77" t="s">
+        <v>38</v>
+      </c>
+      <c r="G77" s="10">
+        <f t="shared" si="21"/>
+        <v>-12230.810000000056</v>
+      </c>
+      <c r="H77" s="10">
+        <f t="shared" si="21"/>
+        <v>-45485.580000000075</v>
+      </c>
+      <c r="I77" s="10">
+        <f t="shared" si="21"/>
+        <v>-72.879999999888241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>-8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>-1724.9000000000233</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F78" t="s">
+        <v>39</v>
+      </c>
+      <c r="G78" s="10">
+        <f t="shared" si="21"/>
+        <v>-4950.4699999999721</v>
+      </c>
+      <c r="H78" s="10">
+        <f t="shared" si="21"/>
+        <v>-8005.7900000010268</v>
+      </c>
+      <c r="I78" s="10">
+        <f t="shared" si="21"/>
+        <v>-1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>55</v>
       </c>
       <c r="B79">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-184239.79000001028</v>
       </c>
       <c r="C79">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>-133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
+        <v>-82077.349999999627</v>
+      </c>
+      <c r="F79" t="s">
+        <v>55</v>
+      </c>
+      <c r="G79" s="10">
+        <f t="shared" si="21"/>
+        <v>-184239.79000001028</v>
+      </c>
+      <c r="H79" s="10">
+        <f t="shared" si="21"/>
+        <v>-133456.33000001032</v>
+      </c>
+      <c r="I79" s="10">
+        <f t="shared" si="21"/>
         <v>-82077.349999999627</v>
       </c>
     </row>

</xml_diff>